<commit_message>
update the calculation excel file
</commit_message>
<xml_diff>
--- a/documents/firmware calculation.xlsx
+++ b/documents/firmware calculation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Temporary\MCP19215\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MCP19215-ADM00799\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FA135A-9130-48F6-A8B3-667CC8A2F813}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DC1312-46D3-4888-8C00-92B408B4B072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93020CC2-5CBA-4B12-846F-691E3D039D97}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>R3</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>OVLO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Band Gap Voltage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -157,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +190,13 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -220,20 +239,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -289,8 +311,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6115050" y="120015"/>
-          <a:ext cx="9068952" cy="6509334"/>
+          <a:off x="6991350" y="120015"/>
+          <a:ext cx="9068952" cy="6440754"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -643,31 +665,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2D39F5-DB12-44E6-8FA3-AA9A4D176B52}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="1">
@@ -722,7 +744,7 @@
       </c>
       <c r="B4" s="1">
         <f>B1*(B3/(B2+B3))</f>
-        <v>1.5950920245398772</v>
+        <v>0.95705521472392641</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -764,7 +786,7 @@
       </c>
       <c r="B6" s="1">
         <f>(B4*1000)/(B5/(2^8))</f>
-        <v>199.38650306748465</v>
+        <v>119.6319018404908</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -774,8 +796,24 @@
         <v>50.000000000000007</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B4/4.096*1024</f>
+        <v>239.2638036809816</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <f>(F4+2.048)/4.096*1024</f>
+        <v>562</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="1">
@@ -784,7 +822,7 @@
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="1">
@@ -892,7 +930,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1">
@@ -912,7 +950,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="1">
@@ -929,6 +967,26 @@
       <c r="B26" s="1">
         <f>LOG((B25/7.4847),1.0286)</f>
         <v>24.653277966798118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1">
+        <f>B28/4.096*1024</f>
+        <v>307.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>